<commit_message>
agregando horario del dia, posible dia disponible, base de interfaz de logueo
</commit_message>
<xml_diff>
--- a/Cypher_Vault/Horarios Disponibles - Alejandro.xlsx
+++ b/Cypher_Vault/Horarios Disponibles - Alejandro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27618"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moras\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javier\StudioProjects\TP_Labo_Principal\Cypher_Vault\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201809C0-F87C-4CC3-B6D5-5ABA93C57C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E13A398-57DF-4264-800A-4149D369B104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11310" xr2:uid="{D6E6CA37-37D6-4C7C-8C58-3258484FDD53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D6E6CA37-37D6-4C7C-8C58-3258484FDD53}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="21">
   <si>
     <t>Lunes</t>
   </si>
@@ -62,9 +51,6 @@
     <t>HORAS DEL DIA</t>
   </si>
   <si>
-    <t>Alejandro</t>
-  </si>
-  <si>
     <t>No disponible</t>
   </si>
   <si>
@@ -72,13 +58,147 @@
   </si>
   <si>
     <t>Disponible</t>
+  </si>
+  <si>
+    <r>
+      <t>Alejandro/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="6"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Javier</t>
+    </r>
+  </si>
+  <si>
+    <t>Alejandro/Javier</t>
+  </si>
+  <si>
+    <t>Alejandro/javier</t>
+  </si>
+  <si>
+    <r>
+      <t>Alejandro/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>javier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Alejandro/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Javier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Alejandro/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Javier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Alejandro/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="6"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>javier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Alejandro/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>javier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Alejandro/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>javier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Alejandro/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="9"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Javier</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +249,22 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="6"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -548,7 +684,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -588,25 +724,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -614,25 +750,25 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -640,25 +776,25 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -666,25 +802,25 @@
         <v>0.125</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -692,25 +828,25 @@
         <v>0.16666666666666699</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -718,25 +854,25 @@
         <v>0.20833333333333301</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -744,25 +880,25 @@
         <v>0.25</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -770,25 +906,25 @@
         <v>0.29166666666666702</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -796,25 +932,25 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -827,25 +963,25 @@
         <v>0.375</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
@@ -858,25 +994,25 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -889,25 +1025,25 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -920,25 +1056,25 @@
         <v>0.5</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -951,25 +1087,25 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
@@ -982,25 +1118,25 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1008,25 +1144,25 @@
         <v>0.625</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1034,25 +1170,25 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1060,25 +1196,25 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1086,25 +1222,25 @@
         <v>0.75</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1112,25 +1248,25 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1138,25 +1274,25 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1164,25 +1300,25 @@
         <v>0.875</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1190,25 +1326,25 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1216,25 +1352,25 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1243,19 +1379,19 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>